<commit_message>
make generate bar color a reusable function
</commit_message>
<xml_diff>
--- a/transaction3.xlsx
+++ b/transaction3.xlsx
@@ -432,6 +432,210 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$D$2:$D$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$D$2:$D$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <dPt>
+            <idx val="0"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="#9F9C12"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="1"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="#09BFB6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <dPt>
+            <idx val="2"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="#DB5BEF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$D$2:$D$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -495,6 +699,72 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="6" name="Chart 6"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>

</xml_diff>